<commit_message>
add time-domain simulation for IEEE-14
</commit_message>
<xml_diff>
--- a/modified_ieee_14/IEEE_14Bus_Cyprus_modified.xlsx
+++ b/modified_ieee_14/IEEE_14Bus_Cyprus_modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\Simplus-Grid-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Simplus-Grid-Tool\modified_ieee_14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B01279C-D96E-4566-A7E8-BE03A7968624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AFE9F6-66F5-411A-9484-55DAA4977279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="28800" windowHeight="15540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -887,11 +887,11 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1514,29 +1514,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:AW18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="3" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="3" width="29.54296875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" customWidth="1"/>
     <col min="8" max="8" width="26" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" customWidth="1"/>
-    <col min="47" max="47" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7265625" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" customWidth="1"/>
+    <col min="12" max="12" width="17.1796875" customWidth="1"/>
+    <col min="13" max="13" width="17.81640625" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" customWidth="1"/>
+    <col min="15" max="15" width="13.1796875" customWidth="1"/>
+    <col min="17" max="17" width="11.26953125" customWidth="1"/>
+    <col min="18" max="18" width="12.81640625" customWidth="1"/>
+    <col min="47" max="47" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49">
@@ -1544,7 +1544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:49" ht="30">
+    <row r="2" spans="1:49" ht="29">
       <c r="A2" s="3"/>
       <c r="B2" s="12" t="s">
         <v>92</v>
@@ -1667,7 +1667,7 @@
       <c r="AV3" s="17"/>
       <c r="AW3" s="19"/>
     </row>
-    <row r="4" spans="1:49" ht="75">
+    <row r="4" spans="1:49" ht="72.5">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="14" t="s">
@@ -2617,12 +2617,12 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2678,10 +2678,10 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2727,11 +2727,11 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3281,13 +3281,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3349,7 +3349,7 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>